<commit_message>
add try and exceptions
</commit_message>
<xml_diff>
--- a/ip_blocked.xlsx
+++ b/ip_blocked.xlsx
@@ -766,14 +766,14 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="L5" t="n">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2023-08-27T13:20:23+00:00</t>
+          <t>2023-08-27T15:13:43+00:00</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2023-08-27T14:01:33+00:00</t>
+          <t>2023-08-27T15:08:47+00:00</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1183,14 +1183,14 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>14275</v>
+        <v>14278</v>
       </c>
       <c r="L11" t="n">
         <v>95</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2023-08-27T14:40:10+00:00</t>
+          <t>2023-08-27T15:04:45+00:00</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1455,14 +1455,14 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="L15" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>2023-08-27T13:50:02+00:00</t>
+          <t>2023-08-27T15:00:03+00:00</t>
         </is>
       </c>
       <c r="N15" t="inlineStr"/>
@@ -1521,7 +1521,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>2999</v>
+        <v>2994</v>
       </c>
       <c r="L16" t="n">
         <v>684</v>
@@ -1591,14 +1591,14 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>1491</v>
+        <v>1493</v>
       </c>
       <c r="L17" t="n">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>2023-08-27T14:22:51+00:00</t>
+          <t>2023-08-27T15:10:18+00:00</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1731,14 +1731,14 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="L19" t="n">
         <v>80</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>2023-08-27T12:53:15+00:00</t>
+          <t>2023-08-27T15:03:37+00:00</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -1867,14 +1867,14 @@
         <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>3038</v>
+        <v>3039</v>
       </c>
       <c r="L21" t="n">
         <v>741</v>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>2023-08-27T14:42:37+00:00</t>
+          <t>2023-08-27T15:13:21+00:00</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -1937,14 +1937,14 @@
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>1063</v>
+        <v>1066</v>
       </c>
       <c r="L22" t="n">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>2023-08-27T14:07:14+00:00</t>
+          <t>2023-08-27T15:05:31+00:00</t>
         </is>
       </c>
       <c r="N22" t="inlineStr"/>

</xml_diff>